<commit_message>
flipping GCONST field to be more friendly to extended addressing modes
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19960" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -2371,7 +2371,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2392,15 +2392,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2605,34 +2596,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2832,59 +2797,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2893,36 +2863,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3022,6 +3004,10 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3121,6 +3107,10 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3452,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3476,12 +3466,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="28" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -3704,7 +3694,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>649</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -3713,7 +3703,7 @@
       <c r="C11" s="22">
         <v>16</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="27" t="s">
         <v>648</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -4226,7 +4216,7 @@
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="31" t="s">
         <v>659</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -4241,12 +4231,10 @@
       <c r="I47" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>612</v>
-      </c>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="33"/>
+      <c r="D48" s="31"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
@@ -4259,9 +4247,12 @@
       <c r="I48" s="19" t="s">
         <v>156</v>
       </c>
+      <c r="L48" s="1" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="33"/>
+      <c r="D49" s="31"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
@@ -4276,7 +4267,7 @@
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="33"/>
+      <c r="D50" s="31"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
@@ -4291,7 +4282,7 @@
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="33"/>
+      <c r="D51" s="31"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
@@ -4306,7 +4297,7 @@
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="33"/>
+      <c r="D52" s="31"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4321,7 +4312,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="33"/>
+      <c r="D53" s="31"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4336,7 +4327,7 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="33"/>
+      <c r="D54" s="31"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
@@ -4541,113 +4532,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I7"/>
+  <dimension ref="A4:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:9" ht="16" thickBot="1"/>
-    <row r="4" spans="1:9" ht="16" thickBot="1">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:9" ht="16" thickBot="1"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" thickBot="1">
-      <c r="A5" s="36" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>654</v>
+      </c>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33" t="s">
         <v>653</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="34" t="s">
-        <v>654</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>615</v>
-      </c>
-      <c r="I5" s="24" t="s">
+      <c r="H6" s="37"/>
+      <c r="I6" s="32" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" thickBot="1">
-      <c r="A6" s="36" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>657</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33" t="s">
         <v>658</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="34" t="s">
-        <v>657</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>616</v>
-      </c>
-      <c r="I6" s="24" t="s">
+      <c r="H7" s="37"/>
+      <c r="I7" s="32" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16" thickBot="1">
-      <c r="A7" s="36">
+    <row r="8" spans="1:9" ht="16" thickBot="1">
+      <c r="A8" s="12">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13">
+        <v>8</v>
+      </c>
+      <c r="D8" s="13">
+        <v>8</v>
+      </c>
+      <c r="E8" s="38">
         <v>16</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="34">
+      <c r="F8" s="38"/>
+      <c r="G8" s="38">
         <v>16</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="22">
-        <v>8</v>
-      </c>
-      <c r="F7" s="22">
-        <v>8</v>
-      </c>
-      <c r="G7" s="22">
-        <v>8</v>
-      </c>
-      <c r="H7" s="23">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H8" s="39"/>
+      <c r="I8" s="32" t="s">
         <v>621</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4660,7 +4652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -4672,28 +4664,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="2"/>

</xml_diff>

<commit_message>
more work on the arch specs; adding fence.ga instruction for a global adddress fence
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="300" yWindow="100" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="673">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2317,6 +2317,18 @@
   </si>
   <si>
     <t>AMO: Compare and Swap</t>
+  </si>
+  <si>
+    <t>FENCE.GA</t>
+  </si>
+  <si>
+    <t>Global Memory Fence</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Bit</t>
   </si>
 </sst>
 </file>
@@ -2597,7 +2609,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="207">
+  <cellStyleXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2805,8 +2817,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2867,6 +2883,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2879,12 +2898,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2892,6 +2905,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2903,8 +2919,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="207">
+  <cellStyles count="211">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3008,6 +3027,8 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3111,6 +3132,8 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3442,7 +3465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
@@ -3466,12 +3489,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -4216,7 +4239,7 @@
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="32" t="s">
         <v>659</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -4234,7 +4257,7 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="31"/>
+      <c r="D48" s="32"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
@@ -4252,7 +4275,7 @@
       </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="31"/>
+      <c r="D49" s="32"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
@@ -4267,7 +4290,7 @@
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="31"/>
+      <c r="D50" s="32"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
@@ -4282,7 +4305,7 @@
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="31"/>
+      <c r="D51" s="32"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
@@ -4297,7 +4320,7 @@
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="31"/>
+      <c r="D52" s="32"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4312,7 +4335,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="31"/>
+      <c r="D53" s="32"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4327,7 +4350,7 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="31"/>
+      <c r="D54" s="32"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
@@ -4532,26 +4555,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I8"/>
+  <dimension ref="A4:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="4" spans="1:9" ht="16" thickBot="1"/>
     <row r="5" spans="1:9">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
@@ -4566,15 +4589,15 @@
       <c r="D6" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="36" t="s">
         <v>654</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33" t="s">
+      <c r="F6" s="36"/>
+      <c r="G6" s="36" t="s">
         <v>653</v>
       </c>
       <c r="H6" s="37"/>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="28" t="s">
         <v>623</v>
       </c>
     </row>
@@ -4591,15 +4614,15 @@
       <c r="D7" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="36" t="s">
         <v>657</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="36" t="s">
         <v>658</v>
       </c>
       <c r="H7" s="37"/>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="28" t="s">
         <v>622</v>
       </c>
     </row>
@@ -4624,12 +4647,56 @@
         <v>16</v>
       </c>
       <c r="H8" s="39"/>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="28" t="s">
         <v>621</v>
       </c>
     </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>671</v>
+      </c>
+      <c r="B11" t="s">
+        <v>672</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="13">
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4652,8 +4719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4664,13 +4731,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="23" t="s">
@@ -5235,7 +5302,7 @@
         <v>156</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>492</v>
@@ -5416,7 +5483,7 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>669</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>156</v>
@@ -5425,7 +5492,7 @@
         <v>156</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>156</v>
+        <v>670</v>
       </c>
     </row>
     <row r="46" spans="1:5">

</xml_diff>

<commit_message>
adding new control register definitions and arch instructions
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="100" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="300" yWindow="100" windowWidth="24020" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="682">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2329,6 +2329,33 @@
   </si>
   <si>
     <t>Bit</t>
+  </si>
+  <si>
+    <t>SPAWN</t>
+  </si>
+  <si>
+    <t>Task Spawn</t>
+  </si>
+  <si>
+    <t>JOIN</t>
+  </si>
+  <si>
+    <t>Task Join</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>GEXC</t>
+  </si>
+  <si>
+    <t>IWAIT</t>
+  </si>
+  <si>
+    <t>Instruction Wait [Hazard]</t>
+  </si>
+  <si>
+    <t>GKEY</t>
   </si>
 </sst>
 </file>
@@ -2609,7 +2636,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="211">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2821,8 +2848,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2886,6 +2921,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2897,6 +2935,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2919,11 +2960,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="211">
+  <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3029,6 +3067,10 @@
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3134,6 +3176,10 @@
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3465,8 +3511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3489,12 +3535,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -4239,7 +4285,7 @@
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="33" t="s">
         <v>659</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -4257,7 +4303,7 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="32"/>
+      <c r="D48" s="33"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
@@ -4275,7 +4321,7 @@
       </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="32"/>
+      <c r="D49" s="33"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
@@ -4290,7 +4336,7 @@
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="32"/>
+      <c r="D50" s="33"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
@@ -4305,14 +4351,14 @@
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="32"/>
+      <c r="D51" s="33"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G51" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="H51" s="7" t="s">
+      <c r="G51" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H51" s="29" t="s">
         <v>156</v>
       </c>
       <c r="I51" s="19" t="s">
@@ -4320,7 +4366,7 @@
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="32"/>
+      <c r="D52" s="33"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4335,7 +4381,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="32"/>
+      <c r="D53" s="33"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4350,18 +4396,18 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="32"/>
+      <c r="D54" s="33"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>156</v>
+      <c r="G54" s="29" t="s">
+        <v>681</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>156</v>
+        <v>681</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="4:9">
@@ -4369,13 +4415,13 @@
         <v>80</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>156</v>
+        <v>678</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>156</v>
+        <v>677</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="4:9">
@@ -4557,7 +4603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
@@ -4565,16 +4611,16 @@
   <sheetData>
     <row r="4" spans="1:9" ht="16" thickBot="1"/>
     <row r="5" spans="1:9">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="35" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
@@ -4589,14 +4635,14 @@
       <c r="D6" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="38" t="s">
         <v>654</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36" t="s">
+      <c r="F6" s="38"/>
+      <c r="G6" s="38" t="s">
         <v>653</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="28" t="s">
         <v>623</v>
       </c>
@@ -4614,14 +4660,14 @@
       <c r="D7" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="38" t="s">
         <v>657</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="38" t="s">
         <v>658</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="28" t="s">
         <v>622</v>
       </c>
@@ -4639,14 +4685,14 @@
       <c r="D8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="40">
         <v>16</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38">
+      <c r="F8" s="40"/>
+      <c r="G8" s="40">
         <v>16</v>
       </c>
-      <c r="H8" s="39"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="28" t="s">
         <v>621</v>
       </c>
@@ -4658,45 +4704,39 @@
       <c r="B11" t="s">
         <v>672</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4704,6 +4744,12 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4719,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:E46"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4731,13 +4777,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="23" t="s">
@@ -4768,7 +4814,7 @@
         <v>156</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>157</v>
@@ -8478,16 +8524,16 @@
         <v>541</v>
       </c>
       <c r="B222" t="s">
-        <v>156</v>
+        <v>673</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>156</v>
+        <v>551</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>156</v>
+        <v>674</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -8495,16 +8541,16 @@
         <v>542</v>
       </c>
       <c r="B223" t="s">
-        <v>156</v>
+        <v>675</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>156</v>
+        <v>637</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>156</v>
+        <v>676</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -8512,16 +8558,16 @@
         <v>543</v>
       </c>
       <c r="B224" t="s">
-        <v>156</v>
+        <v>679</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>156</v>
+        <v>551</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>156</v>
+        <v>680</v>
       </c>
     </row>
     <row r="225" spans="1:5">

</xml_diff>

<commit_message>
adding instructions to kick a given task out of the execution context
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="100" windowWidth="24020" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="320" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="683">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2205,9 +2205,6 @@
     <t>SUBB</t>
   </si>
   <si>
-    <t>Ra.Rb.Rt</t>
-  </si>
-  <si>
     <t>Subtract with Borrow</t>
   </si>
   <si>
@@ -2356,6 +2353,12 @@
   </si>
   <si>
     <t>GKEY</t>
+  </si>
+  <si>
+    <t>PEG</t>
+  </si>
+  <si>
+    <t>Peg the task swith pressure</t>
   </si>
 </sst>
 </file>
@@ -2636,7 +2639,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="219">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2856,8 +2859,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2924,6 +2929,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2935,9 +2943,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2960,8 +2965,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="219">
+  <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3071,6 +3079,7 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3180,6 +3189,7 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3511,7 +3521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -3527,7 +3537,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
@@ -3535,12 +3545,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -3557,7 +3567,7 @@
         <v>347</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>25</v>
@@ -3764,16 +3774,16 @@
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="26" t="s">
+        <v>648</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>649</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>650</v>
       </c>
       <c r="C11" s="22">
         <v>16</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -4285,8 +4295,8 @@
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="33" t="s">
-        <v>659</v>
+      <c r="D47" s="34" t="s">
+        <v>658</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>72</v>
@@ -4303,7 +4313,7 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="33"/>
+      <c r="D48" s="34"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
@@ -4321,7 +4331,7 @@
       </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="33"/>
+      <c r="D49" s="34"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
@@ -4336,7 +4346,7 @@
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="33"/>
+      <c r="D50" s="34"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
@@ -4351,7 +4361,7 @@
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="33"/>
+      <c r="D51" s="34"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
@@ -4366,7 +4376,7 @@
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="33"/>
+      <c r="D52" s="34"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4381,7 +4391,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="33"/>
+      <c r="D53" s="34"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4396,15 +4406,15 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="33"/>
+      <c r="D54" s="34"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>321</v>
@@ -4415,10 +4425,10 @@
         <v>80</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>321</v>
@@ -4516,7 +4526,7 @@
         <v>482</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>321</v>
@@ -4633,14 +4643,14 @@
         <v>615</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="28" t="s">
@@ -4658,14 +4668,14 @@
         <v>616</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="E7" s="38" t="s">
         <v>656</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>657</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H7" s="39"/>
       <c r="I7" s="28" t="s">
@@ -4699,44 +4709,50 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>670</v>
+      </c>
+      <c r="B11" t="s">
         <v>671</v>
       </c>
-      <c r="B11" t="s">
-        <v>672</v>
-      </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4744,12 +4760,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4765,8 +4775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="B224" sqref="B224"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4777,13 +4787,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="23" t="s">
@@ -5257,16 +5267,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5274,7 +5284,7 @@
         <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>173</v>
@@ -5283,7 +5293,7 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5529,16 +5539,16 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
+        <v>668</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6688,7 +6698,7 @@
         <v>139</v>
       </c>
       <c r="B114" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>172</v>
@@ -6697,7 +6707,7 @@
         <v>321</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -8507,16 +8517,16 @@
         <v>540</v>
       </c>
       <c r="B221" t="s">
+        <v>650</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>651</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -8524,7 +8534,7 @@
         <v>541</v>
       </c>
       <c r="B222" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>551</v>
@@ -8533,7 +8543,7 @@
         <v>156</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -8541,16 +8551,16 @@
         <v>542</v>
       </c>
       <c r="B223" t="s">
+        <v>674</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -8558,7 +8568,7 @@
         <v>543</v>
       </c>
       <c r="B224" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>551</v>
@@ -8567,7 +8577,7 @@
         <v>156</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -8575,7 +8585,7 @@
         <v>544</v>
       </c>
       <c r="B225" t="s">
-        <v>156</v>
+        <v>681</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>156</v>
@@ -8584,7 +8594,7 @@
         <v>156</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>156</v>
+        <v>682</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -8662,14 +8672,14 @@
       <c r="B230" t="s">
         <v>630</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="C230" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -8898,7 +8908,7 @@
         <v>583</v>
       </c>
       <c r="B244" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>551</v>
@@ -8907,7 +8917,7 @@
         <v>321</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -8915,16 +8925,16 @@
         <v>584</v>
       </c>
       <c r="B245" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -8932,7 +8942,7 @@
         <v>585</v>
       </c>
       <c r="B246" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>551</v>
@@ -8941,7 +8951,7 @@
         <v>321</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -8949,16 +8959,16 @@
         <v>586</v>
       </c>
       <c r="B247" t="s">
+        <v>635</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>637</v>
-      </c>
       <c r="D247" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -9051,7 +9061,7 @@
         <v>592</v>
       </c>
       <c r="B253" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>172</v>
@@ -9060,7 +9070,7 @@
         <v>321</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -9102,7 +9112,7 @@
         <v>595</v>
       </c>
       <c r="B256" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>172</v>
@@ -9111,7 +9121,7 @@
         <v>321</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -9136,16 +9146,16 @@
         <v>597</v>
       </c>
       <c r="B258" t="s">
+        <v>645</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating instruction definitions for the SEL instructions; the target and comparison type is now annotated in the instruction mneumonic; this makes lazy assemblers much easier
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="320" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="685">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -1745,38 +1745,6 @@
     <t>Memory Fence</t>
   </si>
   <si>
-    <t>SEL</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEL</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.NE,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.EQ,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.GT,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.LT,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.GTE,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC3.LTE,Rt,Rt,Rt</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Select NE to CC3</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -2368,6 +2336,27 @@
   </si>
   <si>
     <t>Future Instruction</t>
+  </si>
+  <si>
+    <t>SEL.CC3.NE</t>
+  </si>
+  <si>
+    <t>SEL.CC3.EQ</t>
+  </si>
+  <si>
+    <t>SEL.CC3.GT</t>
+  </si>
+  <si>
+    <t>SEL.CC3.LT</t>
+  </si>
+  <si>
+    <t>SEL.CC3.GTE</t>
+  </si>
+  <si>
+    <t>SEL.CC3.LTE</t>
+  </si>
+  <si>
+    <t>Rt,Rt,Rt</t>
   </si>
 </sst>
 </file>
@@ -2648,7 +2637,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="221">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2870,8 +2859,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2941,6 +2932,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2952,6 +2946,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2974,11 +2971,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="221">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3089,6 +3083,7 @@
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3199,6 +3194,7 @@
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3546,7 +3542,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
@@ -3554,12 +3550,12 @@
       <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>479</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1">
       <c r="A2" s="9" t="s">
@@ -3576,7 +3572,7 @@
         <v>347</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>25</v>
@@ -3783,16 +3779,16 @@
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="26" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C11" s="22">
         <v>16</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -4190,10 +4186,10 @@
         <v>64</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="I39" s="19" t="s">
         <v>156</v>
@@ -4204,10 +4200,10 @@
         <v>65</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>156</v>
@@ -4218,10 +4214,10 @@
         <v>66</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="I41" s="19" t="s">
         <v>156</v>
@@ -4232,10 +4228,10 @@
         <v>67</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="I42" s="19" t="s">
         <v>156</v>
@@ -4243,16 +4239,16 @@
     </row>
     <row r="43" spans="4:12">
       <c r="D43" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="I43" s="19" t="s">
         <v>156</v>
@@ -4260,16 +4256,16 @@
     </row>
     <row r="44" spans="4:12">
       <c r="D44" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>156</v>
@@ -4280,10 +4276,10 @@
         <v>70</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>156</v>
@@ -4294,27 +4290,27 @@
         <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="47" spans="4:12">
-      <c r="D47" s="34" t="s">
-        <v>658</v>
+      <c r="D47" s="35" t="s">
+        <v>650</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="I47" s="19" t="s">
         <v>156</v>
@@ -4322,55 +4318,55 @@
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="4:12">
-      <c r="D48" s="34"/>
+      <c r="D48" s="35"/>
       <c r="F48" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="I48" s="19" t="s">
         <v>156</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="49" spans="4:9">
-      <c r="D49" s="34"/>
+      <c r="D49" s="35"/>
       <c r="F49" s="6" t="s">
         <v>74</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="I49" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="50" spans="4:9">
-      <c r="D50" s="34"/>
+      <c r="D50" s="35"/>
       <c r="F50" s="6" t="s">
         <v>75</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="51" spans="4:9">
-      <c r="D51" s="34"/>
+      <c r="D51" s="35"/>
       <c r="F51" s="6" t="s">
         <v>76</v>
       </c>
@@ -4385,7 +4381,7 @@
       </c>
     </row>
     <row r="52" spans="4:9">
-      <c r="D52" s="34"/>
+      <c r="D52" s="35"/>
       <c r="F52" s="6" t="s">
         <v>77</v>
       </c>
@@ -4400,7 +4396,7 @@
       </c>
     </row>
     <row r="53" spans="4:9">
-      <c r="D53" s="34"/>
+      <c r="D53" s="35"/>
       <c r="F53" s="6" t="s">
         <v>78</v>
       </c>
@@ -4415,15 +4411,15 @@
       </c>
     </row>
     <row r="54" spans="4:9">
-      <c r="D54" s="34"/>
+      <c r="D54" s="35"/>
       <c r="F54" s="6" t="s">
         <v>79</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>321</v>
@@ -4434,10 +4430,10 @@
         <v>80</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>321</v>
@@ -4535,7 +4531,7 @@
         <v>482</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>321</v>
@@ -4588,10 +4584,10 @@
         <v>91</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>321</v>
@@ -4630,65 +4626,65 @@
   <sheetData>
     <row r="4" spans="1:9" ht="16" thickBot="1"/>
     <row r="5" spans="1:9">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>645</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40" t="s">
+        <v>644</v>
+      </c>
+      <c r="H6" s="41"/>
+      <c r="I6" s="28" t="s">
         <v>615</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>653</v>
-      </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38" t="s">
-        <v>652</v>
-      </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="28" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>656</v>
-      </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38" t="s">
-        <v>657</v>
-      </c>
-      <c r="H7" s="39"/>
+        <v>647</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>648</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40" t="s">
+        <v>649</v>
+      </c>
+      <c r="H7" s="41"/>
       <c r="I7" s="28" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" thickBot="1">
@@ -4704,64 +4700,58 @@
       <c r="D8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="42">
         <v>16</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40">
+      <c r="F8" s="42"/>
+      <c r="G8" s="42">
         <v>16</v>
       </c>
-      <c r="H8" s="41"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="28" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B11" t="s">
-        <v>671</v>
-      </c>
-      <c r="C11" s="42" t="s">
+        <v>663</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4769,6 +4759,12 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4784,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="E226" sqref="E226"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4796,13 +4792,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="16" thickBot="1">
       <c r="A2" s="23" t="s">
@@ -5276,16 +5272,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5293,7 +5289,7 @@
         <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>173</v>
@@ -5302,7 +5298,7 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5548,7 +5544,7 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>156</v>
@@ -5557,7 +5553,7 @@
         <v>156</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6707,7 +6703,7 @@
         <v>139</v>
       </c>
       <c r="B114" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>172</v>
@@ -6716,7 +6712,7 @@
         <v>321</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -6996,7 +6992,7 @@
         <v>348</v>
       </c>
       <c r="B131" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>189</v>
@@ -7005,7 +7001,7 @@
         <v>321</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -7013,7 +7009,7 @@
         <v>349</v>
       </c>
       <c r="B132" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>189</v>
@@ -7022,7 +7018,7 @@
         <v>321</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -7030,7 +7026,7 @@
         <v>350</v>
       </c>
       <c r="B133" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>189</v>
@@ -7039,7 +7035,7 @@
         <v>321</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -7047,7 +7043,7 @@
         <v>351</v>
       </c>
       <c r="B134" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>189</v>
@@ -7056,7 +7052,7 @@
         <v>321</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -7268,7 +7264,7 @@
         <v>364</v>
       </c>
       <c r="B147" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>189</v>
@@ -7277,7 +7273,7 @@
         <v>321</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -7285,7 +7281,7 @@
         <v>365</v>
       </c>
       <c r="B148" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>189</v>
@@ -7294,7 +7290,7 @@
         <v>321</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -7302,7 +7298,7 @@
         <v>366</v>
       </c>
       <c r="B149" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>189</v>
@@ -7311,7 +7307,7 @@
         <v>321</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -7319,7 +7315,7 @@
         <v>367</v>
       </c>
       <c r="B150" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>189</v>
@@ -7328,7 +7324,7 @@
         <v>321</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -7540,16 +7536,16 @@
         <v>380</v>
       </c>
       <c r="B163" t="s">
+        <v>678</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E163" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -7557,16 +7553,16 @@
         <v>381</v>
       </c>
       <c r="B164" t="s">
-        <v>493</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>496</v>
+        <v>679</v>
+      </c>
+      <c r="C164" s="31" t="s">
+        <v>684</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -7574,16 +7570,16 @@
         <v>382</v>
       </c>
       <c r="B165" t="s">
-        <v>493</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>497</v>
+        <v>680</v>
+      </c>
+      <c r="C165" s="31" t="s">
+        <v>684</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -7591,16 +7587,16 @@
         <v>383</v>
       </c>
       <c r="B166" t="s">
-        <v>494</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>498</v>
+        <v>681</v>
+      </c>
+      <c r="C166" s="31" t="s">
+        <v>684</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -7608,16 +7604,16 @@
         <v>384</v>
       </c>
       <c r="B167" t="s">
-        <v>494</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>499</v>
+        <v>682</v>
+      </c>
+      <c r="C167" s="31" t="s">
+        <v>684</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -7625,16 +7621,16 @@
         <v>385</v>
       </c>
       <c r="B168" t="s">
-        <v>494</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>500</v>
+        <v>683</v>
+      </c>
+      <c r="C168" s="31" t="s">
+        <v>684</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -7812,7 +7808,7 @@
         <v>396</v>
       </c>
       <c r="B179" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>156</v>
@@ -7821,7 +7817,7 @@
         <v>156</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -7829,16 +7825,16 @@
         <v>397</v>
       </c>
       <c r="B180" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -7982,16 +7978,16 @@
         <v>406</v>
       </c>
       <c r="B189" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -7999,16 +7995,16 @@
         <v>407</v>
       </c>
       <c r="B190" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -8084,16 +8080,16 @@
         <v>412</v>
       </c>
       <c r="B195" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -8101,16 +8097,16 @@
         <v>413</v>
       </c>
       <c r="B196" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -8254,16 +8250,16 @@
         <v>422</v>
       </c>
       <c r="B205" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="C205" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E205" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -8271,16 +8267,16 @@
         <v>423</v>
       </c>
       <c r="B206" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -8356,38 +8352,38 @@
         <v>428</v>
       </c>
       <c r="B211" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="B212" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="B213" t="s">
         <v>156</v>
@@ -8404,7 +8400,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="1" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B214" t="s">
         <v>156</v>
@@ -8421,7 +8417,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B215" t="s">
         <v>156</v>
@@ -8438,7 +8434,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="B216" t="s">
         <v>156</v>
@@ -8455,7 +8451,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B217" t="s">
         <v>156</v>
@@ -8472,7 +8468,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B218" t="s">
         <v>156</v>
@@ -8489,7 +8485,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B219" t="s">
         <v>156</v>
@@ -8506,7 +8502,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="B220" t="s">
         <v>156</v>
@@ -8523,78 +8519,78 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="B221" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="B222" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="B223" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B224" t="s">
+        <v>670</v>
+      </c>
+      <c r="C224" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="B224" t="s">
-        <v>678</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>551</v>
-      </c>
       <c r="D224" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B225" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>156</v>
@@ -8603,29 +8599,29 @@
         <v>156</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="B226" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="B227" t="s">
         <v>304</v>
@@ -8642,10 +8638,10 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B228" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>172</v>
@@ -8654,12 +8650,12 @@
         <v>321</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B229" t="s">
         <v>156</v>
@@ -8676,10 +8672,10 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="B230" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="C230" s="30" t="s">
         <v>172</v>
@@ -8688,12 +8684,12 @@
         <v>321</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="B231" t="s">
         <v>156</v>
@@ -8710,10 +8706,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="B232" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>172</v>
@@ -8722,12 +8718,12 @@
         <v>321</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B233" t="s">
         <v>156</v>
@@ -8744,7 +8740,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="B234" t="s">
         <v>156</v>
@@ -8761,7 +8757,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="B235" t="s">
         <v>156</v>
@@ -8778,7 +8774,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B236" t="s">
         <v>156</v>
@@ -8795,7 +8791,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B237" t="s">
         <v>305</v>
@@ -8812,7 +8808,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="B238" t="s">
         <v>306</v>
@@ -8829,7 +8825,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="B239" t="s">
         <v>307</v>
@@ -8846,7 +8842,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="B240" t="s">
         <v>156</v>
@@ -8863,7 +8859,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="B241" t="s">
         <v>156</v>
@@ -8880,7 +8876,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B242" t="s">
         <v>156</v>
@@ -8897,7 +8893,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="B243" t="s">
         <v>156</v>
@@ -8914,75 +8910,75 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="B244" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B245" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="B246" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="B247" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="B248" t="s">
         <v>156</v>
@@ -8999,7 +8995,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B249" t="s">
         <v>156</v>
@@ -9016,7 +9012,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B250" t="s">
         <v>156</v>
@@ -9033,7 +9029,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="B251" t="s">
         <v>156</v>
@@ -9050,7 +9046,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="B252" t="s">
         <v>156</v>
@@ -9067,10 +9063,10 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="B253" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>172</v>
@@ -9079,12 +9075,12 @@
         <v>321</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="B254" t="s">
         <v>156</v>
@@ -9101,7 +9097,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="B255" t="s">
         <v>156</v>
@@ -9118,10 +9114,10 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B256" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>172</v>
@@ -9130,12 +9126,12 @@
         <v>321</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B257" t="s">
         <v>156</v>
@@ -9152,19 +9148,19 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="B258" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating instruction mneumonics to make instruction parsing easier and instruction definitions more clear
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="689">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -1955,10 +1955,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>CALL</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Call</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -2357,6 +2353,21 @@
   </si>
   <si>
     <t>Rt,Rt,Rt</t>
+  </si>
+  <si>
+    <t>RTNA</t>
+  </si>
+  <si>
+    <t>BRC</t>
+  </si>
+  <si>
+    <t>BRAC</t>
+  </si>
+  <si>
+    <t>CALLC</t>
+  </si>
+  <si>
+    <t>CALLAC</t>
   </si>
 </sst>
 </file>
@@ -2947,9 +2958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2969,6 +2977,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3542,7 +3553,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
@@ -3572,7 +3583,7 @@
         <v>347</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>25</v>
@@ -3779,16 +3790,16 @@
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1">
       <c r="A11" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>640</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>641</v>
       </c>
       <c r="C11" s="22">
         <v>16</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>36</v>
@@ -4239,7 +4250,7 @@
     </row>
     <row r="43" spans="4:12">
       <c r="D43" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>68</v>
@@ -4256,16 +4267,16 @@
     </row>
     <row r="44" spans="4:12">
       <c r="D44" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G44" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>592</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>593</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>156</v>
@@ -4276,10 +4287,10 @@
         <v>70</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>156</v>
@@ -4290,10 +4301,10 @@
         <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>156</v>
@@ -4301,16 +4312,16 @@
     </row>
     <row r="47" spans="4:12">
       <c r="D47" s="35" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G47" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="H47" s="7" t="s">
         <v>616</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>617</v>
       </c>
       <c r="I47" s="19" t="s">
         <v>156</v>
@@ -4323,16 +4334,16 @@
         <v>73</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>591</v>
-      </c>
       <c r="I48" s="19" t="s">
         <v>156</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="49" spans="4:9">
@@ -4341,10 +4352,10 @@
         <v>74</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I49" s="19" t="s">
         <v>156</v>
@@ -4356,10 +4367,10 @@
         <v>75</v>
       </c>
       <c r="G50" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>605</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>606</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>156</v>
@@ -4416,10 +4427,10 @@
         <v>79</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>321</v>
@@ -4430,10 +4441,10 @@
         <v>80</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>321</v>
@@ -4531,7 +4542,7 @@
         <v>482</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>321</v>
@@ -4584,10 +4595,10 @@
         <v>91</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>321</v>
@@ -4626,65 +4637,65 @@
   <sheetData>
     <row r="4" spans="1:9" ht="16" thickBot="1"/>
     <row r="5" spans="1:9">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="E6" s="40" t="s">
         <v>645</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40" t="s">
+      <c r="E6" s="39" t="s">
         <v>644</v>
       </c>
-      <c r="H6" s="41"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39" t="s">
+        <v>643</v>
+      </c>
+      <c r="H6" s="40"/>
       <c r="I6" s="28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="E7" s="39" t="s">
         <v>647</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="F7" s="39"/>
+      <c r="G7" s="39" t="s">
         <v>648</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40" t="s">
-        <v>649</v>
-      </c>
-      <c r="H7" s="41"/>
+      <c r="H7" s="40"/>
       <c r="I7" s="28" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" thickBot="1">
@@ -4700,58 +4711,64 @@
       <c r="D8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>16</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42">
+      <c r="F8" s="41"/>
+      <c r="G8" s="41">
         <v>16</v>
       </c>
-      <c r="H8" s="43"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="28" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>661</v>
+      </c>
+      <c r="B11" t="s">
         <v>662</v>
       </c>
-      <c r="B11" t="s">
-        <v>663</v>
-      </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4759,12 +4776,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4780,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5272,16 +5283,16 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5289,7 +5300,7 @@
         <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>173</v>
@@ -5298,7 +5309,7 @@
         <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5544,16 +5555,16 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
+        <v>659</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6703,7 +6714,7 @@
         <v>139</v>
       </c>
       <c r="B114" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>172</v>
@@ -6712,7 +6723,7 @@
         <v>321</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -7536,10 +7547,10 @@
         <v>380</v>
       </c>
       <c r="B163" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>321</v>
@@ -7553,10 +7564,10 @@
         <v>381</v>
       </c>
       <c r="B164" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>321</v>
@@ -7570,10 +7581,10 @@
         <v>382</v>
       </c>
       <c r="B165" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>321</v>
@@ -7587,10 +7598,10 @@
         <v>383</v>
       </c>
       <c r="B166" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>321</v>
@@ -7604,10 +7615,10 @@
         <v>384</v>
       </c>
       <c r="B167" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>321</v>
@@ -7621,10 +7632,10 @@
         <v>385</v>
       </c>
       <c r="B168" t="s">
+        <v>682</v>
+      </c>
+      <c r="C168" s="31" t="s">
         <v>683</v>
-      </c>
-      <c r="C168" s="31" t="s">
-        <v>684</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>321</v>
@@ -7825,7 +7836,7 @@
         <v>397</v>
       </c>
       <c r="B180" t="s">
-        <v>538</v>
+        <v>684</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>543</v>
@@ -7995,10 +8006,10 @@
         <v>407</v>
       </c>
       <c r="B190" t="s">
-        <v>544</v>
+        <v>685</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>156</v>
@@ -8097,10 +8108,10 @@
         <v>413</v>
       </c>
       <c r="B196" t="s">
-        <v>548</v>
+        <v>686</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>156</v>
@@ -8259,7 +8270,7 @@
         <v>156</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -8267,16 +8278,16 @@
         <v>423</v>
       </c>
       <c r="B206" t="s">
-        <v>552</v>
+        <v>687</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -8352,7 +8363,7 @@
         <v>428</v>
       </c>
       <c r="B211" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>545</v>
@@ -8361,7 +8372,7 @@
         <v>156</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -8369,16 +8380,16 @@
         <v>523</v>
       </c>
       <c r="B212" t="s">
+        <v>688</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C212" s="1" t="s">
-        <v>556</v>
-      </c>
       <c r="D212" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -8522,16 +8533,16 @@
         <v>532</v>
       </c>
       <c r="B221" t="s">
+        <v>641</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -8539,7 +8550,7 @@
         <v>533</v>
       </c>
       <c r="B222" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>543</v>
@@ -8548,7 +8559,7 @@
         <v>156</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -8556,16 +8567,16 @@
         <v>534</v>
       </c>
       <c r="B223" t="s">
+        <v>665</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E223" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -8573,7 +8584,7 @@
         <v>535</v>
       </c>
       <c r="B224" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>543</v>
@@ -8582,7 +8593,7 @@
         <v>156</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -8590,16 +8601,16 @@
         <v>536</v>
       </c>
       <c r="B225" t="s">
+        <v>672</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E225" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -8607,21 +8618,21 @@
         <v>537</v>
       </c>
       <c r="B226" t="s">
+        <v>674</v>
+      </c>
+      <c r="C226" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="C226" s="1" t="s">
+      <c r="D226" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E226" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B227" t="s">
         <v>304</v>
@@ -8638,10 +8649,10 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B228" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>172</v>
@@ -8650,12 +8661,12 @@
         <v>321</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B229" t="s">
         <v>156</v>
@@ -8672,10 +8683,10 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B230" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C230" s="30" t="s">
         <v>172</v>
@@ -8684,12 +8695,12 @@
         <v>321</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B231" t="s">
         <v>156</v>
@@ -8706,10 +8717,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B232" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>172</v>
@@ -8718,12 +8729,12 @@
         <v>321</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B233" t="s">
         <v>156</v>
@@ -8740,7 +8751,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B234" t="s">
         <v>156</v>
@@ -8757,7 +8768,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B235" t="s">
         <v>156</v>
@@ -8774,7 +8785,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B236" t="s">
         <v>156</v>
@@ -8791,7 +8802,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B237" t="s">
         <v>305</v>
@@ -8808,7 +8819,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B238" t="s">
         <v>306</v>
@@ -8825,7 +8836,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B239" t="s">
         <v>307</v>
@@ -8842,7 +8853,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B240" t="s">
         <v>156</v>
@@ -8859,7 +8870,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B241" t="s">
         <v>156</v>
@@ -8876,7 +8887,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B242" t="s">
         <v>156</v>
@@ -8893,7 +8904,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B243" t="s">
         <v>156</v>
@@ -8910,10 +8921,10 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B244" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>543</v>
@@ -8922,32 +8933,32 @@
         <v>321</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B245" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D245" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B246" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>543</v>
@@ -8956,29 +8967,29 @@
         <v>321</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B247" t="s">
+        <v>626</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>628</v>
-      </c>
       <c r="D247" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B248" t="s">
         <v>156</v>
@@ -8995,7 +9006,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B249" t="s">
         <v>156</v>
@@ -9012,7 +9023,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B250" t="s">
         <v>156</v>
@@ -9029,7 +9040,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B251" t="s">
         <v>156</v>
@@ -9046,7 +9057,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B252" t="s">
         <v>156</v>
@@ -9063,10 +9074,10 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B253" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>172</v>
@@ -9075,12 +9086,12 @@
         <v>321</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B254" t="s">
         <v>156</v>
@@ -9097,7 +9108,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B255" t="s">
         <v>156</v>
@@ -9114,10 +9125,10 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B256" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>172</v>
@@ -9126,12 +9137,12 @@
         <v>321</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B257" t="s">
         <v>156</v>
@@ -9148,19 +9159,19 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B258" t="s">
+        <v>636</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating IP register definition
</commit_message>
<xml_diff>
--- a/doc/goblin-core_opcodes.xlsx
+++ b/doc/goblin-core_opcodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="320" windowWidth="24020" windowHeight="14660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="800" yWindow="320" windowWidth="24020" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="691">
   <si>
     <t>Unsigned Byte</t>
   </si>
@@ -2368,6 +2368,12 @@
   </si>
   <si>
     <t>CALLAC</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Instruction Pointer</t>
   </si>
 </sst>
 </file>
@@ -2958,6 +2964,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2977,9 +2986,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3537,8 +3543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4382,10 +4388,10 @@
         <v>76</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>156</v>
+        <v>689</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>156</v>
+        <v>690</v>
       </c>
       <c r="I51" s="19" t="s">
         <v>156</v>
@@ -4637,16 +4643,16 @@
   <sheetData>
     <row r="4" spans="1:9" ht="16" thickBot="1"/>
     <row r="5" spans="1:9">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
@@ -4661,14 +4667,14 @@
       <c r="D6" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="40" t="s">
         <v>644</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="40" t="s">
         <v>643</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="28" t="s">
         <v>614</v>
       </c>
@@ -4686,14 +4692,14 @@
       <c r="D7" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="40" t="s">
         <v>647</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39" t="s">
+      <c r="F7" s="40"/>
+      <c r="G7" s="40" t="s">
         <v>648</v>
       </c>
-      <c r="H7" s="40"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="28" t="s">
         <v>613</v>
       </c>
@@ -4711,14 +4717,14 @@
       <c r="D8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="42">
         <v>16</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41">
+      <c r="F8" s="42"/>
+      <c r="G8" s="42">
         <v>16</v>
       </c>
-      <c r="H8" s="42"/>
+      <c r="H8" s="43"/>
       <c r="I8" s="28" t="s">
         <v>612</v>
       </c>
@@ -4730,45 +4736,39 @@
       <c r="B11" t="s">
         <v>662</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4776,6 +4776,12 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4791,7 +4797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+    <sheetView topLeftCell="A195" workbookViewId="0">
       <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>

</xml_diff>